<commit_message>
Changed graph to degrees for more clarity
</commit_message>
<xml_diff>
--- a/rgbd-slam/docs/OdometryDataSet.xlsx
+++ b/rgbd-slam/docs/OdometryDataSet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="660" windowWidth="28260" windowHeight="17180" tabRatio="500"/>
+    <workbookView xWindow="720" yWindow="20" windowWidth="28260" windowHeight="17180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="29">
   <si>
     <t>Ground truth</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>C MS T</t>
+  </si>
+  <si>
+    <t>rad to degree</t>
   </si>
 </sst>
 </file>
@@ -736,13 +739,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0071675698113099</c:v>
+                  <c:v>0.410671493486658</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0495192509434461</c:v>
+                  <c:v>2.837244041794565</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.146731222597646</c:v>
+                  <c:v>8.407079653443398</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1312,13 +1315,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0071675698113099</c:v>
+                  <c:v>0.410671493486658</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0495192509434461</c:v>
+                  <c:v>2.837244041794565</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.146731222597646</c:v>
+                  <c:v>8.407079653443398</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1365,22 +1368,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0324201174118786</c:v>
+                  <c:v>1.857535871578181</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.106630334056496</c:v>
+                  <c:v>6.109468019253214</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0924232217032063</c:v>
+                  <c:v>5.295460454366708</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.107730249609847</c:v>
+                  <c:v>6.172488537350023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18368079128205</c:v>
+                  <c:v>10.52413396261361</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.184248017101949</c:v>
+                  <c:v>10.55663360764455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1460,7 +1463,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Error (radians)</a:t>
+                  <a:t> Error (degrees)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -2004,8 +2007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="M111" workbookViewId="0">
-      <selection activeCell="Z26" sqref="Z26"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="K12" workbookViewId="0">
+      <selection activeCell="Q46" sqref="Q46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2589,28 +2592,28 @@
         <v>20</v>
       </c>
       <c r="AA7">
-        <f>SQRT(S6*S6+S7*S7+S8*S8)</f>
-        <v>3.2420117411878613E-2</v>
+        <f>$Y$11*SQRT(S6*S6+S7*S7+S8*S8)</f>
+        <v>1.8575358715781809</v>
       </c>
       <c r="AB7">
-        <f t="shared" ref="AB7:AF7" si="4">SQRT(T6*T6+T7*T7+T8*T8)</f>
-        <v>0.10663033405649644</v>
+        <f t="shared" ref="AB7:AF7" si="4">$Y$11*SQRT(T6*T6+T7*T7+T8*T8)</f>
+        <v>6.1094680192532147</v>
       </c>
       <c r="AC7">
         <f t="shared" si="4"/>
-        <v>9.2423221703206285E-2</v>
+        <v>5.2954604543667081</v>
       </c>
       <c r="AD7">
         <f t="shared" si="4"/>
-        <v>0.10773024960984727</v>
+        <v>6.1724885373500227</v>
       </c>
       <c r="AE7">
         <f t="shared" si="4"/>
-        <v>0.18368079128205</v>
+        <v>10.524133962613615</v>
       </c>
       <c r="AF7">
         <f t="shared" si="4"/>
-        <v>0.18424801710194882</v>
+        <v>10.556633607644553</v>
       </c>
       <c r="AH7" t="s">
         <v>24</v>
@@ -2697,33 +2700,36 @@
       </c>
       <c r="AB8">
         <f>SQRT((AB7-AA7)*(AB7-AA7))</f>
-        <v>7.4210216644617827E-2</v>
+        <v>4.251932147675034</v>
       </c>
       <c r="AC8">
         <f t="shared" ref="AC8:AF8" si="5">SQRT((AC7-AB7)*(AC7-AB7))</f>
-        <v>1.4207112353290155E-2</v>
+        <v>0.81400756488650661</v>
       </c>
       <c r="AD8">
         <f t="shared" si="5"/>
-        <v>1.5307027906640985E-2</v>
+        <v>0.87702808298331458</v>
       </c>
       <c r="AE8">
         <f t="shared" si="5"/>
-        <v>7.5950541672202734E-2</v>
+        <v>4.3516454252635919</v>
       </c>
       <c r="AF8">
         <f t="shared" si="5"/>
-        <v>5.6722581989882004E-4</v>
+        <v>3.2499645030938495E-2</v>
       </c>
       <c r="AH8">
         <f>AVERAGE(AB8/AB4,AC8/AC4,AD8/AD4,AE8/AE4,AF8/AF4)</f>
-        <v>7.1845094548384631E-4</v>
+        <v>4.1164206355296259E-2</v>
       </c>
     </row>
     <row r="10" spans="1:34">
       <c r="B10" t="s">
         <v>7</v>
       </c>
+      <c r="Y10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:34">
       <c r="B11" t="s">
@@ -2738,6 +2744,10 @@
       <c r="E11">
         <v>1.5707960000000001</v>
       </c>
+      <c r="Y11">
+        <f>180/3.1415927</f>
+        <v>57.295778666661661</v>
+      </c>
     </row>
     <row r="12" spans="1:34">
       <c r="B12" t="s">
@@ -3033,20 +3043,20 @@
         <v>20</v>
       </c>
       <c r="R19">
-        <f>SQRT(H19*H19+H20*H20+H21*H21)</f>
-        <v>7.1675698113099042E-3</v>
+        <f>$Y$11*SQRT(H19*H19+H20*H20+H21*H21)</f>
+        <v>0.41067149348665816</v>
       </c>
       <c r="S19">
-        <f>SQRT(I19*I19+I20*I20+I21*I21)</f>
-        <v>4.9519250943446114E-2</v>
+        <f t="shared" ref="S19:T19" si="6">$Y$11*SQRT(I19*I19+I20*I20+I21*I21)</f>
+        <v>2.8372440417945652</v>
       </c>
       <c r="T19">
-        <f>SQRT(J19*J19+J20*J20+J21*J21)</f>
-        <v>0.14673122259764615</v>
+        <f t="shared" si="6"/>
+        <v>8.4070796534433985</v>
       </c>
       <c r="V19">
         <f>AVERAGE(S20/S18,T20/T18)</f>
-        <v>1.5651666741887742E-4</v>
+        <v>8.9677443340754961E-3</v>
       </c>
     </row>
     <row r="20" spans="2:22">
@@ -3097,11 +3107,11 @@
       </c>
       <c r="S20">
         <f>S19-R19</f>
-        <v>4.2351681132136207E-2</v>
+        <v>2.4265725483079073</v>
       </c>
       <c r="T20">
         <f>T19-S19</f>
-        <v>9.7211971654200036E-2</v>
+        <v>5.5698356116488332</v>
       </c>
     </row>
     <row r="21" spans="2:22">

</xml_diff>